<commit_message>
Added new split tmsd + dbl purification designs and streamlined echo command generator
Also added new dbl purification sequences to P3518_MA
</commit_message>
<xml_diff>
--- a/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/cargo_plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67A50B94-0755-4C92-B4C4-AAA26506E4CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E45F1EE-C1E6-5E4E-81F5-2E9FEAA5477A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-4450" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
     <sheet name="Names" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="180">
   <si>
     <t>1</t>
   </si>
@@ -539,13 +539,109 @@
   </si>
   <si>
     <t>biotin-anchor_id17_*</t>
+  </si>
+  <si>
+    <r>
+      <t>CTTGAAAACATAGATGATGAAACAAAACAAAtt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CTCTTATTAC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CCAAATTCTCCTTACACATTC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GGGCGCCAGGGTGCTGGTTTGCCCCAGCAGGTTCCAGTTTGGttCCAAATTCTCCTTACACATTC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CTCTTATTAC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CTTGAAAACATAGATGATGAAACAAAACAAAttCCAAATTCTCCTTACACATTCCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CTTATTAC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GGGCGCCAGGGTGCTGGTTTGCCCCAGCAGGTTCCAGTTTGGtt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CTCTTATTAC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CCAAATTCTCCTTACACATTC</t>
+    </r>
+  </si>
+  <si>
+    <t>Anchor Sequence (Wiggum Core, 10-base Flanders Toehold) on Slat Handle 1, H2, with design ID outer_toehold</t>
+  </si>
+  <si>
+    <t>Anchor Sequence (Wiggum Core, 10-base Flanders Toehold) on Slat Handle 32, H2, with design ID outer_toehold</t>
+  </si>
+  <si>
+    <t>Anchor Sequence (Wiggum Core, 10-base Flanders Toehold) on Slat Handle 1, H2, with design ID inner_toehold</t>
+  </si>
+  <si>
+    <t>Anchor Sequence (Wiggum Core, 10-base Flanders Toehold) on Slat Handle 32, H2, with design ID inner_toehold</t>
+  </si>
+  <si>
+    <t>Anchor-Wiggum-Flanders-outer-toehold_h2_pos1</t>
+  </si>
+  <si>
+    <t>Anchor-Wiggum-Flanders-outer-toehold_h2_pos32</t>
+  </si>
+  <si>
+    <t>Anchor-Wiggum-Flanders-inner-toehold_h2_pos1</t>
+  </si>
+  <si>
+    <t>Anchor-Wiggum-Flanders-inner-toehold_h2_pos32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,12 +653,18 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -913,13 +1015,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="95" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -996,7 +1104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1031,7 +1139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1174,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1113,7 +1221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1139,7 +1247,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -1147,57 +1255,69 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
@@ -1211,18 +1331,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.15625" customWidth="1"/>
-    <col min="2" max="15" width="30.1015625" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="15" width="30.1640625" customWidth="1"/>
     <col min="16" max="25" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>166</v>
       </c>
@@ -1299,7 +1419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1348,7 +1468,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1397,7 +1517,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1454,7 +1574,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1497,7 +1617,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -1528,14 +1648,22 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1557,7 +1685,7 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
@@ -1586,7 +1714,7 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -1615,7 +1743,7 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -1644,7 +1772,7 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -1673,7 +1801,7 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -1702,7 +1830,7 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1731,7 +1859,7 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -1760,7 +1888,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
@@ -1789,7 +1917,7 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
@@ -1818,7 +1946,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
@@ -1857,12 +1985,12 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -1939,7 +2067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1974,7 +2102,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -2009,7 +2137,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -2056,7 +2184,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2082,7 +2210,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -2090,57 +2218,69 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Added new bionwire 'wide trench' design, fixed bug in new handle library plates and updated cargo plate
</commit_message>
<xml_diff>
--- a/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E45F1EE-C1E6-5E4E-81F5-2E9FEAA5477A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD2BFDD-87D9-894F-8DC7-C252F1C9A500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Names" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="201">
   <si>
     <t>1</t>
   </si>
@@ -635,6 +635,69 @@
   </si>
   <si>
     <t>Anchor-Wiggum-Flanders-inner-toehold_h2_pos32</t>
+  </si>
+  <si>
+    <t>AACCTCCCGTTTTTGTTTAACGTCAAAAGATGGCAATTCATCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>CATCCTAATTCCGGTATTCTAAGAACGCTTCTGAATAATGGAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>GGCAAGGCATAGGTAAAGATTCAAAAGGCCGCCAGCCATTGCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>CTTTACAGAGAAGCCCTTTTTAAGAAAACCAGAAGGAGCGGAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h5_pos27</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h2_pos8</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h2_pos23</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h5_pos28</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h2_pos6</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h5_pos11</t>
+  </si>
+  <si>
+    <t>GoldWireBinder_h5_pos26</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 27 on side 5.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 8 on side 2.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 23 on side 2.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 28 on side 5.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 6 on side 2.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 11 on side 5.</t>
+  </si>
+  <si>
+    <t>Binding handle for the BioNWire gold nanowires at position 26 on side 5.</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="67" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="67" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1276,6 +1339,27 @@
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="B8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1324,6 +1408,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1332,7 +1417,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1689,13 +1774,27 @@
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" t="s">
+        <v>193</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1984,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2239,6 +2338,27 @@
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">

</xml_diff>

<commit_message>
Updated sequence for bionwire wide trench design
</commit_message>
<xml_diff>
--- a/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD2BFDD-87D9-894F-8DC7-C252F1C9A500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9722E1D-7867-D741-9434-F16BFD46DD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -637,27 +637,6 @@
     <t>Anchor-Wiggum-Flanders-inner-toehold_h2_pos32</t>
   </si>
   <si>
-    <t>AACCTCCCGTTTTTGTTTAACGTCAAAAGATGGCAATTCATCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>CATCCTAATTCCGGTATTCTAAGAACGCTTCTGAATAATGGAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>GGCAAGGCATAGGTAAAGATTCAAAAGGCCGCCAGCCATTGCttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
-    <t>CTTTACAGAGAAGCCCTTTTTAAGAAAACCAGAAGGAGCGGAttTTTTGGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
-  </si>
-  <si>
     <t>GoldWireBinder_h5_pos27</t>
   </si>
   <si>
@@ -698,6 +677,27 @@
   </si>
   <si>
     <t>Binding handle for the BioNWire gold nanowires at position 26 on side 5.</t>
+  </si>
+  <si>
+    <t>CATCCTAATTCCGGTATTCTAAGAACGCTTCTGAATAATGGAttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>GGCAAGGCATAGGTAAAGATTCAAAAGGCCGCCAGCCATTGCttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>GAAACAATCGGCAAGAGACGCAGAAACAGCCGCACAGGCGGCttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>TCAACATTAAATGGCGCATCGTAACCGTGCGGAAACCAGGCAttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>TAGCAAGGCCGGCGTTTTCATCGGCATTTTCAGAGCCGCCACttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>AACCTCCCGTTTTTGTTTAACGTCAAAAGATGGCAATTCATCttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
+  </si>
+  <si>
+    <t>CTTTACAGAGAAGCCCTTTTTAAGAAAACCAGAAGGAGCGGAttGGTTGATAAAAGCATGACAGGTTGATAATATAGAT</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1340,25 +1340,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="G8" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="H8" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -1416,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1775,25 +1775,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G8" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2083,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2339,25 +2339,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E8" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="G8" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="H8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated bionwire sequence gen system to be deterministic
</commit_message>
<xml_diff>
--- a/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/cargo_plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9722E1D-7867-D741-9434-F16BFD46DD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70756D4-6F71-7E4B-9F49-16CB1F522D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1340,25 +1340,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" t="s">
         <v>194</v>
       </c>
-      <c r="C8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>196</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>197</v>
-      </c>
-      <c r="F8" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" t="s">
-        <v>199</v>
-      </c>
-      <c r="H8" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:H8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1775,25 +1775,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" t="s">
         <v>183</v>
       </c>
-      <c r="C8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>184</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>181</v>
-      </c>
-      <c r="F8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G8" t="s">
-        <v>180</v>
-      </c>
-      <c r="H8" t="s">
-        <v>186</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2083,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2339,25 +2339,25 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" t="s">
         <v>190</v>
       </c>
-      <c r="C8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>191</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>188</v>
-      </c>
-      <c r="F8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>